<commit_message>
added (not 100% operational) loading from excel collection, fetching all cards from scryfall and fetching edhrec data for all cards
</commit_message>
<xml_diff>
--- a/collection/test_100.xlsx
+++ b/collection/test_100.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles-Alexis\Documents\edhrecEnhanced\collection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEDD303-5724-443B-AEF4-B2D07537F3A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8228EF5-4527-40FA-88DA-B480675A3DD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -977,11 +977,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G103"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>